<commit_message>
More work on my thesis. Test on Agile
</commit_message>
<xml_diff>
--- a/JPADSandBox/out/Wing airfoil data BOEING/data.xlsx
+++ b/JPADSandBox/out/Wing airfoil data BOEING/data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="30">
   <si>
     <t>Airfoil Tip</t>
   </si>
@@ -74,15 +74,51 @@
   <si>
     <t>α = 24</t>
   </si>
+  <si>
+    <t xml:space="preserve">Philipps </t>
+  </si>
+  <si>
+    <t>CL max</t>
+  </si>
+  <si>
+    <t>Mod.</t>
+  </si>
+  <si>
+    <t>Mod. Stall Path II</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CL_max</t>
+  </si>
+  <si>
+    <t>α_stall</t>
+  </si>
+  <si>
+    <t>CL_max</t>
+  </si>
+  <si>
+    <t>Calculated Values</t>
+  </si>
+  <si>
+    <t>Ref. Values (CFD)</t>
+  </si>
+  <si>
+    <t>Results</t>
+  </si>
+  <si>
+    <t>Erros (%)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.0000000"/>
+    <numFmt numFmtId="166" formatCode="0.000000000"/>
+    <numFmt numFmtId="167" formatCode="0.00000000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -113,8 +149,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -155,8 +205,31 @@
         <bgColor theme="4" tint="0.79998168889431442"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor theme="5" tint="0.59999389629810485"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor theme="5" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -204,8 +277,58 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="5" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="5" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="5" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="5" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="5" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="5" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -213,8 +336,11 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -223,16 +349,10 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="5" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="4" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="3" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="4" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="5" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="6" applyAlignment="1">
@@ -241,20 +361,52 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="4"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="8" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="5" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="7"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="9"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="10">
+    <cellStyle name="20% - Colore 2" xfId="8" builtinId="34"/>
+    <cellStyle name="40% - Colore 1" xfId="7" builtinId="31"/>
     <cellStyle name="60% - Colore 1" xfId="3" builtinId="32"/>
     <cellStyle name="60% - Colore 2" xfId="5" builtinId="36"/>
     <cellStyle name="Colore 1" xfId="2" builtinId="29"/>
     <cellStyle name="Colore 2" xfId="4" builtinId="33"/>
+    <cellStyle name="Colore 6" xfId="9" builtinId="49"/>
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
     <cellStyle name="Titolo 1" xfId="6" builtinId="16"/>
     <cellStyle name="Titolo 3" xfId="1" builtinId="18"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="7">
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.00000000"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.0000"/>
     </dxf>
@@ -667,11 +819,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="197813248"/>
-        <c:axId val="196945600"/>
+        <c:axId val="195548160"/>
+        <c:axId val="219917696"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="197813248"/>
+        <c:axId val="195548160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -694,14 +846,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="196945600"/>
+        <c:crossAx val="219917696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -709,7 +860,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="196945600"/>
+        <c:axId val="219917696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -732,21 +883,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="197813248"/>
+        <c:crossAx val="195548160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1353,11 +1502,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="126982144"/>
-        <c:axId val="139667136"/>
+        <c:axId val="195547136"/>
+        <c:axId val="219919424"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="126982144"/>
+        <c:axId val="195547136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1387,7 +1536,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="139667136"/>
+        <c:crossAx val="219919424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1395,7 +1544,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="139667136"/>
+        <c:axId val="219919424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1425,7 +1574,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="126982144"/>
+        <c:crossAx val="195547136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1623,11 +1772,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="197815296"/>
-        <c:axId val="196949056"/>
+        <c:axId val="195550720"/>
+        <c:axId val="219921728"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="197815296"/>
+        <c:axId val="195550720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1637,7 +1786,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="196949056"/>
+        <c:crossAx val="219921728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1645,7 +1794,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="196949056"/>
+        <c:axId val="219921728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2.5"/>
@@ -1658,7 +1807,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="197815296"/>
+        <c:crossAx val="195550720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.2"/>
@@ -1877,11 +2026,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="197814784"/>
-        <c:axId val="196950784"/>
+        <c:axId val="226988544"/>
+        <c:axId val="230106240"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="197814784"/>
+        <c:axId val="226988544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1891,7 +2040,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="196950784"/>
+        <c:crossAx val="230106240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1899,7 +2048,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="196950784"/>
+        <c:axId val="230106240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1910,7 +2059,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="197814784"/>
+        <c:crossAx val="226988544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2251,11 +2400,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="197814272"/>
-        <c:axId val="198484544"/>
+        <c:axId val="226959360"/>
+        <c:axId val="230107968"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="197814272"/>
+        <c:axId val="226959360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2265,7 +2414,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="198484544"/>
+        <c:crossAx val="230107968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2273,7 +2422,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="198484544"/>
+        <c:axId val="230107968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2284,7 +2433,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="197814272"/>
+        <c:crossAx val="226959360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2814,6 +2963,152 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>Mod. Stall Path II</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Foglio1!$AG$54:$AG$73</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>-6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>24</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Foglio1!$AH$54:$AH$73</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>-0.15101315691</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.39936114593511901</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.1331935497299299</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.2249226002042799</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.270787125</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="0.00000000">
+                  <c:v>1.3157701295937501</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="0.00000000">
+                  <c:v>1.4002826109062501</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="0.00000000">
+                  <c:v>1.4771580429687501</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="0.00000000">
+                  <c:v>1.5459576112812501</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="0.00000000">
+                  <c:v>1.60624250134375</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="0.00000000">
+                  <c:v>1.65757389865625</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="0.00000000">
+                  <c:v>1.6995129887187499</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="0.00000000">
+                  <c:v>1.73162095703124</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="0.00000000">
+                  <c:v>1.75345898909374</c:v>
+                </c:pt>
+                <c:pt idx="14" formatCode="0.00000000">
+                  <c:v>1.7645882704062399</c:v>
+                </c:pt>
+                <c:pt idx="15" formatCode="0.00000000">
+                  <c:v>1.7645699864687501</c:v>
+                </c:pt>
+                <c:pt idx="16" formatCode="0.00000000">
+                  <c:v>1.7529653227812401</c:v>
+                </c:pt>
+                <c:pt idx="17" formatCode="0.00000000">
+                  <c:v>1.72933546484375</c:v>
+                </c:pt>
+                <c:pt idx="18" formatCode="0.00000000">
+                  <c:v>1.6932415981562401</c:v>
+                </c:pt>
+                <c:pt idx="19" formatCode="0.00000000">
+                  <c:v>1.64424490821875</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -2822,11 +3117,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="198486272"/>
-        <c:axId val="198486848"/>
+        <c:axId val="230109696"/>
+        <c:axId val="230110272"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="198486272"/>
+        <c:axId val="230109696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2837,13 +3132,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="198486848"/>
+        <c:crossAx val="230110272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="198486848"/>
+        <c:axId val="230110272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2854,7 +3149,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="198486272"/>
+        <c:crossAx val="230109696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.2"/>
@@ -2898,6 +3193,284 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
+          <c:x val="0.23268823666479835"/>
+          <c:y val="3.9748223300268795E-2"/>
+          <c:w val="0.7356906756826056"/>
+          <c:h val="0.85536943609753291"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Foglio1!$Y$54:$Y$72</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>-6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>24</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Foglio1!$Z$54:$Z$72</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>-0.15101315691</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.39936114593511901</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.1331935497299299</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.2249226002042799</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.3170606568779999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.410248161433</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.500792212618</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.5844933565449999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.657152139326</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.7145691070710001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.7525448058919999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.7668797818990001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.753374581204</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.7078297499170001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.626045834151</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.503823380017</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.3369629336240001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.121265041085</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.85253024851100001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Foglio1!$AO$54:$AO$56</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Foglio1!$AP$54:$AP$56</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.39936114593511901</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.1331935497299299</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.8670259535247409</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="226811200"/>
+        <c:axId val="226810624"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="226811200"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:minorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="226810624"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="1"/>
+        <c:minorUnit val="1"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="226810624"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:minorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="226811200"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="it-IT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
           <c:x val="6.3628975225579448E-2"/>
           <c:y val="5.5263880421482274E-2"/>
           <c:w val="0.85969504260183893"/>
@@ -4426,11 +4999,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="175693824"/>
-        <c:axId val="198489152"/>
+        <c:axId val="195547648"/>
+        <c:axId val="230112576"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="175693824"/>
+        <c:axId val="195547648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4440,7 +5013,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="198489152"/>
+        <c:crossAx val="230112576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4448,7 +5021,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="198489152"/>
+        <c:axId val="230112576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4459,14 +5032,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="175693824"/>
+        <c:crossAx val="195547648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4663,6 +5235,36 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>41903</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>134470</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>47</xdr:col>
+      <xdr:colOff>588308</xdr:colOff>
+      <xdr:row>99</xdr:row>
+      <xdr:rowOff>112058</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Grafico 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4702,11 +5304,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabella3" displayName="Tabella3" ref="A4:B22" totalsRowShown="0" headerRowDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabella3" displayName="Tabella3" ref="A4:B22" totalsRowShown="0" headerRowDxfId="6">
   <autoFilter ref="A4:B22"/>
   <tableColumns count="2">
     <tableColumn id="1" name="α"/>
-    <tableColumn id="2" name="cl" dataDxfId="4"/>
+    <tableColumn id="2" name="cl" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4739,7 +5341,7 @@
   <autoFilter ref="V53:W69"/>
   <tableColumns count="2">
     <tableColumn id="1" name="α"/>
-    <tableColumn id="2" name="CL" dataDxfId="0">
+    <tableColumn id="2" name="CL" dataDxfId="1">
       <calculatedColumnFormula>S54*2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4769,8 +5371,19 @@
 </table>
 </file>
 
+<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabella1" displayName="Tabella1" ref="AG53:AH73" totalsRowShown="0">
+  <autoFilter ref="AG53:AH73"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="α"/>
+    <tableColumn id="2" name="CL" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabella4" displayName="Tabella4" ref="D4:E22" totalsRowShown="0" headerRowDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabella4" displayName="Tabella4" ref="D4:E22" totalsRowShown="0" headerRowDxfId="4">
   <autoFilter ref="D4:E22"/>
   <tableColumns count="2">
     <tableColumn id="1" name="α"/>
@@ -4784,7 +5397,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabella5" displayName="Tabella5" ref="J4:K22" totalsRowShown="0">
   <autoFilter ref="J4:K22"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="α" dataDxfId="2"/>
+    <tableColumn id="1" name="α" dataDxfId="3"/>
     <tableColumn id="2" name="cl"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -4795,7 +5408,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabella6" displayName="Tabella6" ref="M4:N22" totalsRowShown="0">
   <autoFilter ref="M4:N22"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="α" dataDxfId="1"/>
+    <tableColumn id="1" name="α" dataDxfId="2"/>
     <tableColumn id="2" name="cl"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -5144,111 +5757,117 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE72"/>
+  <dimension ref="A1:AP92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J46" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="V51" sqref="V51:AC51"/>
+    <sheetView tabSelected="1" topLeftCell="M66" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AI97" sqref="AI97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="33" max="33" width="10.1328125" customWidth="1"/>
+    <col min="34" max="34" width="13.06640625" customWidth="1"/>
+    <col min="35" max="35" width="15.86328125" customWidth="1"/>
+    <col min="40" max="40" width="12.1328125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="19.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="R1" s="10" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="R1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="S1" s="10"/>
-      <c r="T1" s="10"/>
-      <c r="U1" s="10"/>
-      <c r="V1" s="10"/>
-      <c r="W1" s="10"/>
-      <c r="X1" s="10"/>
-      <c r="Y1" s="10"/>
-      <c r="Z1" s="10"/>
-      <c r="AA1" s="10"/>
-      <c r="AB1" s="10"/>
-      <c r="AC1" s="10"/>
-      <c r="AD1" s="10"/>
-      <c r="AE1" s="10"/>
+      <c r="S1" s="8"/>
+      <c r="T1" s="8"/>
+      <c r="U1" s="8"/>
+      <c r="V1" s="8"/>
+      <c r="W1" s="8"/>
+      <c r="X1" s="8"/>
+      <c r="Y1" s="8"/>
+      <c r="Z1" s="8"/>
+      <c r="AA1" s="8"/>
+      <c r="AB1" s="8"/>
+      <c r="AC1" s="8"/>
+      <c r="AD1" s="8"/>
+      <c r="AE1" s="8"/>
     </row>
     <row r="2" spans="1:31" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="J2" s="7" t="s">
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="J2" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-      <c r="R2" s="11" t="s">
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="11"/>
+      <c r="R2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="S2" s="11"/>
-      <c r="T2" s="11"/>
-      <c r="U2" s="11"/>
-      <c r="V2" s="11"/>
-      <c r="AA2" s="11" t="s">
+      <c r="S2" s="9"/>
+      <c r="T2" s="9"/>
+      <c r="U2" s="9"/>
+      <c r="V2" s="9"/>
+      <c r="AA2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="AB2" s="11"/>
-      <c r="AC2" s="11"/>
-      <c r="AD2" s="11"/>
-      <c r="AE2" s="11"/>
+      <c r="AB2" s="9"/>
+      <c r="AC2" s="9"/>
+      <c r="AD2" s="9"/>
+      <c r="AE2" s="9"/>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.45">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="D3" s="8" t="s">
+      <c r="B3" s="10"/>
+      <c r="D3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="8"/>
-      <c r="J3" s="8" t="s">
+      <c r="E3" s="10"/>
+      <c r="J3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="K3" s="8"/>
-      <c r="M3" s="8" t="s">
+      <c r="K3" s="10"/>
+      <c r="M3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="N3" s="8"/>
-      <c r="R3" s="8" t="s">
+      <c r="N3" s="10"/>
+      <c r="R3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="S3" s="8"/>
-      <c r="U3" s="8" t="s">
+      <c r="S3" s="10"/>
+      <c r="U3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="V3" s="8"/>
-      <c r="AA3" s="8" t="s">
+      <c r="V3" s="10"/>
+      <c r="AA3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="AB3" s="8"/>
-      <c r="AD3" s="8" t="s">
+      <c r="AB3" s="10"/>
+      <c r="AD3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="AE3" s="8"/>
+      <c r="AE3" s="10"/>
     </row>
     <row r="4" spans="1:31" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A4" s="5" t="s">
@@ -6219,55 +6838,68 @@
     <row r="25" spans="1:31" x14ac:dyDescent="0.45">
       <c r="B25" s="1"/>
     </row>
-    <row r="51" spans="5:31" x14ac:dyDescent="0.45">
-      <c r="V51" s="9" t="s">
+    <row r="51" spans="5:42" x14ac:dyDescent="0.45">
+      <c r="V51" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="W51" s="9"/>
-      <c r="X51" s="9"/>
-      <c r="Y51" s="9"/>
-      <c r="Z51" s="9"/>
-      <c r="AA51" s="9"/>
-      <c r="AB51" s="9"/>
-      <c r="AC51" s="9"/>
-    </row>
-    <row r="52" spans="5:31" x14ac:dyDescent="0.45">
-      <c r="E52" s="9" t="s">
+      <c r="W51" s="6"/>
+      <c r="X51" s="6"/>
+      <c r="Y51" s="6"/>
+      <c r="Z51" s="6"/>
+      <c r="AA51" s="6"/>
+      <c r="AB51" s="6"/>
+      <c r="AC51" s="6"/>
+      <c r="AD51" s="6"/>
+      <c r="AE51" s="6"/>
+      <c r="AF51" s="6"/>
+      <c r="AG51" s="6"/>
+      <c r="AH51" s="6"/>
+      <c r="AI51" s="6"/>
+    </row>
+    <row r="52" spans="5:42" x14ac:dyDescent="0.45">
+      <c r="E52" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F52" s="9"/>
-      <c r="G52" s="9"/>
-      <c r="H52" s="9"/>
-      <c r="I52" s="9"/>
-      <c r="J52" s="9"/>
-      <c r="K52" s="9"/>
-      <c r="L52" s="9"/>
-      <c r="V52" s="6" t="s">
+      <c r="F52" s="6"/>
+      <c r="G52" s="6"/>
+      <c r="H52" s="6"/>
+      <c r="I52" s="6"/>
+      <c r="J52" s="6"/>
+      <c r="K52" s="6"/>
+      <c r="L52" s="6"/>
+      <c r="V52" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="W52" s="6"/>
-      <c r="Y52" s="6" t="s">
+      <c r="W52" s="7"/>
+      <c r="Y52" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="Z52" s="6"/>
-      <c r="AB52" s="6" t="s">
+      <c r="Z52" s="7"/>
+      <c r="AB52" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="AC52" s="6"/>
-    </row>
-    <row r="53" spans="5:31" x14ac:dyDescent="0.45">
-      <c r="E53" s="6" t="s">
+      <c r="AC52" s="7"/>
+      <c r="AE52" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="AG52" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="AH52" s="7"/>
+    </row>
+    <row r="53" spans="5:42" x14ac:dyDescent="0.45">
+      <c r="E53" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="F53" s="6"/>
-      <c r="H53" s="6" t="s">
+      <c r="F53" s="7"/>
+      <c r="H53" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I53" s="6"/>
-      <c r="K53" s="6" t="s">
+      <c r="I53" s="7"/>
+      <c r="K53" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="L53" s="6"/>
+      <c r="L53" s="7"/>
       <c r="V53" t="s">
         <v>4</v>
       </c>
@@ -6286,8 +6918,17 @@
       <c r="AC53" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="54" spans="5:31" x14ac:dyDescent="0.45">
+      <c r="AE53" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="AG53" t="s">
+        <v>4</v>
+      </c>
+      <c r="AH53" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="54" spans="5:42" x14ac:dyDescent="0.45">
       <c r="E54" t="s">
         <v>4</v>
       </c>
@@ -6331,8 +6972,24 @@
       <c r="AE54">
         <v>1.83</v>
       </c>
-    </row>
-    <row r="55" spans="5:31" x14ac:dyDescent="0.45">
+      <c r="AG54">
+        <v>-6</v>
+      </c>
+      <c r="AH54">
+        <v>-0.15101315691</v>
+      </c>
+      <c r="AJ54">
+        <f>(AP55-AP54)/AO55</f>
+        <v>9.172905047435137E-2</v>
+      </c>
+      <c r="AO54" s="17">
+        <v>0</v>
+      </c>
+      <c r="AP54" s="18">
+        <v>0.39936114593511901</v>
+      </c>
+    </row>
+    <row r="55" spans="5:42" x14ac:dyDescent="0.45">
       <c r="E55">
         <v>0</v>
       </c>
@@ -6384,8 +7041,24 @@
       <c r="AE55">
         <v>1.83</v>
       </c>
-    </row>
-    <row r="56" spans="5:31" x14ac:dyDescent="0.45">
+      <c r="AG55">
+        <v>0</v>
+      </c>
+      <c r="AH55">
+        <v>0.39936114593511901</v>
+      </c>
+      <c r="AJ55">
+        <f>AJ54*57.3</f>
+        <v>5.2560745921803331</v>
+      </c>
+      <c r="AO55" s="14">
+        <v>8</v>
+      </c>
+      <c r="AP55" s="15">
+        <v>1.1331935497299299</v>
+      </c>
+    </row>
+    <row r="56" spans="5:42" x14ac:dyDescent="0.45">
       <c r="E56">
         <v>8</v>
       </c>
@@ -6429,8 +7102,21 @@
       <c r="AE56">
         <v>1.83</v>
       </c>
-    </row>
-    <row r="57" spans="5:31" x14ac:dyDescent="0.45">
+      <c r="AG56">
+        <v>8</v>
+      </c>
+      <c r="AH56">
+        <v>1.1331935497299299</v>
+      </c>
+      <c r="AO56">
+        <v>16</v>
+      </c>
+      <c r="AP56">
+        <f>((AP55-AP54)/AO55)*AO56+AP54</f>
+        <v>1.8670259535247409</v>
+      </c>
+    </row>
+    <row r="57" spans="5:42" x14ac:dyDescent="0.45">
       <c r="E57">
         <v>16</v>
       </c>
@@ -6474,8 +7160,21 @@
       <c r="AE57">
         <v>1.83</v>
       </c>
-    </row>
-    <row r="58" spans="5:31" x14ac:dyDescent="0.45">
+      <c r="AG57">
+        <v>9</v>
+      </c>
+      <c r="AH57">
+        <v>1.2249226002042799</v>
+      </c>
+      <c r="AO57">
+        <v>12.5</v>
+      </c>
+      <c r="AP57">
+        <f>((AP55-AP54)/AO55)*AO57+AP54</f>
+        <v>1.5459742768645111</v>
+      </c>
+    </row>
+    <row r="58" spans="5:42" x14ac:dyDescent="0.45">
       <c r="E58">
         <v>18</v>
       </c>
@@ -6516,8 +7215,21 @@
       <c r="AC58">
         <v>1.2958326477</v>
       </c>
-    </row>
-    <row r="59" spans="5:31" x14ac:dyDescent="0.45">
+      <c r="AG58">
+        <v>9.5</v>
+      </c>
+      <c r="AH58">
+        <v>1.270787125</v>
+      </c>
+      <c r="AO58">
+        <v>10.5</v>
+      </c>
+      <c r="AP58">
+        <f>((AP55-AP54)/AO55)*AO58+AP54</f>
+        <v>1.3625161759158084</v>
+      </c>
+    </row>
+    <row r="59" spans="5:42" x14ac:dyDescent="0.45">
       <c r="E59">
         <v>20</v>
       </c>
@@ -6558,8 +7270,14 @@
       <c r="AC59">
         <v>1.3854858431999999</v>
       </c>
-    </row>
-    <row r="60" spans="5:31" x14ac:dyDescent="0.45">
+      <c r="AG59">
+        <v>10</v>
+      </c>
+      <c r="AH59" s="25">
+        <v>1.3157701295937501</v>
+      </c>
+    </row>
+    <row r="60" spans="5:42" x14ac:dyDescent="0.45">
       <c r="E60">
         <v>22</v>
       </c>
@@ -6600,8 +7318,14 @@
       <c r="AC60">
         <v>1.47281341437</v>
       </c>
-    </row>
-    <row r="61" spans="5:31" x14ac:dyDescent="0.45">
+      <c r="AG60">
+        <v>11</v>
+      </c>
+      <c r="AH60" s="25">
+        <v>1.4002826109062501</v>
+      </c>
+    </row>
+    <row r="61" spans="5:42" x14ac:dyDescent="0.45">
       <c r="E61">
         <v>24</v>
       </c>
@@ -6642,8 +7366,14 @@
       <c r="AC61">
         <v>1.5562337037</v>
       </c>
-    </row>
-    <row r="62" spans="5:31" x14ac:dyDescent="0.45">
+      <c r="AG61">
+        <v>12</v>
+      </c>
+      <c r="AH61" s="25">
+        <v>1.4771580429687501</v>
+      </c>
+    </row>
+    <row r="62" spans="5:42" x14ac:dyDescent="0.45">
       <c r="S62">
         <v>0.64997350112149899</v>
       </c>
@@ -6666,8 +7396,18 @@
       <c r="AC62">
         <v>1.6339169166</v>
       </c>
-    </row>
-    <row r="63" spans="5:31" x14ac:dyDescent="0.45">
+      <c r="AG62" s="13">
+        <v>13</v>
+      </c>
+      <c r="AH62" s="25">
+        <v>1.5459576112812501</v>
+      </c>
+      <c r="AI62" s="23"/>
+      <c r="AN62" s="24">
+        <v>5.8904664723032399E-4</v>
+      </c>
+    </row>
+    <row r="63" spans="5:42" x14ac:dyDescent="0.45">
       <c r="S63">
         <v>0.71547457592319996</v>
       </c>
@@ -6690,8 +7430,18 @@
       <c r="AC63">
         <v>1.7039157402</v>
       </c>
-    </row>
-    <row r="64" spans="5:31" x14ac:dyDescent="0.45">
+      <c r="AG63" s="16">
+        <v>14</v>
+      </c>
+      <c r="AH63" s="25">
+        <v>1.60624250134375</v>
+      </c>
+      <c r="AI63" s="23"/>
+      <c r="AN63" s="24">
+        <v>-3.48263104956269E-2</v>
+      </c>
+    </row>
+    <row r="64" spans="5:42" x14ac:dyDescent="0.45">
       <c r="S64">
         <v>0.76919395781170496</v>
       </c>
@@ -6714,8 +7464,18 @@
       <c r="AC64">
         <v>1.76418194439</v>
       </c>
-    </row>
-    <row r="65" spans="19:29" x14ac:dyDescent="0.45">
+      <c r="AG64" s="13">
+        <v>15</v>
+      </c>
+      <c r="AH64" s="25">
+        <v>1.65757389865625</v>
+      </c>
+      <c r="AI64" s="23"/>
+      <c r="AN64" s="24">
+        <v>0.68627114650145904</v>
+      </c>
+    </row>
+    <row r="65" spans="19:40" x14ac:dyDescent="0.45">
       <c r="S65">
         <v>0.81197170479303205</v>
       </c>
@@ -6738,8 +7498,18 @@
       <c r="AC65">
         <v>1.8126775615299999</v>
       </c>
-    </row>
-    <row r="66" spans="19:29" x14ac:dyDescent="0.45">
+      <c r="AG65" s="16">
+        <v>16</v>
+      </c>
+      <c r="AH65" s="25">
+        <v>1.6995129887187499</v>
+      </c>
+      <c r="AI65" s="23"/>
+      <c r="AN65" s="24">
+        <v>-2.7412900491982501</v>
+      </c>
+    </row>
+    <row r="66" spans="19:40" x14ac:dyDescent="0.45">
       <c r="S66">
         <v>0.84173098526349399</v>
       </c>
@@ -6762,8 +7532,14 @@
       <c r="AC66">
         <v>1.8472690539500001</v>
       </c>
-    </row>
-    <row r="67" spans="19:29" x14ac:dyDescent="0.45">
+      <c r="AG66" s="13">
+        <v>17</v>
+      </c>
+      <c r="AH66" s="25">
+        <v>1.73162095703124</v>
+      </c>
+    </row>
+    <row r="67" spans="19:40" x14ac:dyDescent="0.45">
       <c r="S67">
         <v>0.85193905101120704</v>
       </c>
@@ -6786,8 +7562,14 @@
       <c r="AC67">
         <v>1.86583027299</v>
       </c>
-    </row>
-    <row r="68" spans="19:29" x14ac:dyDescent="0.45">
+      <c r="AG67" s="16">
+        <v>18</v>
+      </c>
+      <c r="AH67" s="25">
+        <v>1.75345898909374</v>
+      </c>
+    </row>
+    <row r="68" spans="19:40" x14ac:dyDescent="0.45">
       <c r="S68">
         <v>0.76231783320889801</v>
       </c>
@@ -6810,8 +7592,14 @@
       <c r="AC68">
         <v>1.8662691091700001</v>
       </c>
-    </row>
-    <row r="69" spans="19:29" x14ac:dyDescent="0.45">
+      <c r="AG68" s="13">
+        <v>19</v>
+      </c>
+      <c r="AH68" s="25">
+        <v>1.7645882704062399</v>
+      </c>
+    </row>
+    <row r="69" spans="19:40" x14ac:dyDescent="0.45">
       <c r="S69">
         <v>0.63193852427340802</v>
       </c>
@@ -6834,8 +7622,14 @@
       <c r="AC69">
         <v>1.84642330191</v>
       </c>
-    </row>
-    <row r="70" spans="19:29" x14ac:dyDescent="0.45">
+      <c r="AG69" s="16">
+        <v>20</v>
+      </c>
+      <c r="AH69" s="25">
+        <v>1.7645699864687501</v>
+      </c>
+    </row>
+    <row r="70" spans="19:40" x14ac:dyDescent="0.45">
       <c r="Y70">
         <v>22</v>
       </c>
@@ -6848,8 +7642,14 @@
       <c r="AC70">
         <v>1.80412542935</v>
       </c>
-    </row>
-    <row r="71" spans="19:29" x14ac:dyDescent="0.45">
+      <c r="AG70" s="13">
+        <v>21</v>
+      </c>
+      <c r="AH70" s="25">
+        <v>1.7529653227812401</v>
+      </c>
+    </row>
+    <row r="71" spans="19:40" x14ac:dyDescent="0.45">
       <c r="Y71">
         <v>23</v>
       </c>
@@ -6862,8 +7662,14 @@
       <c r="AC71">
         <v>1.7372080696000001</v>
       </c>
-    </row>
-    <row r="72" spans="19:29" x14ac:dyDescent="0.45">
+      <c r="AG71" s="16">
+        <v>22</v>
+      </c>
+      <c r="AH71" s="25">
+        <v>1.72933546484375</v>
+      </c>
+    </row>
+    <row r="72" spans="19:40" x14ac:dyDescent="0.45">
       <c r="Y72">
         <v>24</v>
       </c>
@@ -6876,10 +7682,233 @@
       <c r="AC72">
         <v>1.6435038008</v>
       </c>
+      <c r="AG72" s="13">
+        <v>23</v>
+      </c>
+      <c r="AH72" s="25">
+        <v>1.6932415981562401</v>
+      </c>
+    </row>
+    <row r="73" spans="19:40" x14ac:dyDescent="0.45">
+      <c r="AG73" s="19">
+        <v>24</v>
+      </c>
+      <c r="AH73" s="25">
+        <v>1.64424490821875</v>
+      </c>
+    </row>
+    <row r="74" spans="19:40" x14ac:dyDescent="0.45">
+      <c r="AH74" s="25"/>
+    </row>
+    <row r="75" spans="19:40" x14ac:dyDescent="0.45">
+      <c r="Y75" s="20"/>
+      <c r="Z75" s="20"/>
+      <c r="AA75" s="20"/>
+      <c r="AB75" s="20"/>
+      <c r="AC75" s="20"/>
+      <c r="AD75" s="20"/>
+      <c r="AH75" s="25"/>
+    </row>
+    <row r="76" spans="19:40" x14ac:dyDescent="0.45">
+      <c r="Y76" s="20"/>
+      <c r="Z76" s="20"/>
+      <c r="AA76" s="20"/>
+      <c r="AB76" s="20"/>
+      <c r="AC76" s="20"/>
+      <c r="AD76" s="20"/>
+    </row>
+    <row r="77" spans="19:40" x14ac:dyDescent="0.45">
+      <c r="Y77" s="20"/>
+      <c r="Z77" s="20"/>
+      <c r="AA77" s="20"/>
+      <c r="AB77" s="20"/>
+      <c r="AC77" s="20"/>
+      <c r="AD77" s="20"/>
+    </row>
+    <row r="78" spans="19:40" x14ac:dyDescent="0.45">
+      <c r="Y78" s="20"/>
+      <c r="Z78" s="20"/>
+      <c r="AA78" s="20"/>
+      <c r="AB78" s="20"/>
+      <c r="AC78" s="20"/>
+      <c r="AD78" s="20"/>
+    </row>
+    <row r="79" spans="19:40" x14ac:dyDescent="0.45">
+      <c r="Y79" s="20"/>
+      <c r="Z79" s="20"/>
+      <c r="AA79" s="20"/>
+      <c r="AB79" s="20"/>
+      <c r="AC79" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD79" s="6"/>
+      <c r="AE79" s="6"/>
+      <c r="AF79" s="6"/>
+      <c r="AG79" s="6"/>
+      <c r="AH79" s="6"/>
+      <c r="AI79" s="6"/>
+    </row>
+    <row r="80" spans="19:40" x14ac:dyDescent="0.45">
+      <c r="Y80" s="20"/>
+      <c r="Z80" s="20"/>
+      <c r="AA80" s="20"/>
+      <c r="AB80" s="20"/>
+      <c r="AC80" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD80" s="7"/>
+      <c r="AE80" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF80" s="27"/>
+      <c r="AH80" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="AI80" s="29"/>
+    </row>
+    <row r="81" spans="27:35" x14ac:dyDescent="0.45">
+      <c r="AA81" s="20"/>
+      <c r="AB81" s="20"/>
+      <c r="AC81" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="AD81" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE81" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="AF81" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="AH81" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="AI81" s="28" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="82" spans="27:35" x14ac:dyDescent="0.45">
+      <c r="AA82" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB82" s="26"/>
+      <c r="AC82" s="20">
+        <v>17</v>
+      </c>
+      <c r="AD82" s="20">
+        <v>1.766</v>
+      </c>
+      <c r="AE82" s="12">
+        <v>19.600000000000001</v>
+      </c>
+      <c r="AF82" s="12">
+        <v>1.6990000000000001</v>
+      </c>
+      <c r="AH82">
+        <f>(AE82-AC82)/AE82*100</f>
+        <v>13.265306122448987</v>
+      </c>
+      <c r="AI82">
+        <f>(AD82-AF82)/AF82*100</f>
+        <v>3.9434961742201264</v>
+      </c>
+    </row>
+    <row r="83" spans="27:35" x14ac:dyDescent="0.45">
+      <c r="AA83" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB83" s="26"/>
+      <c r="AC83">
+        <v>19.5</v>
+      </c>
+      <c r="AD83">
+        <v>1.766</v>
+      </c>
+      <c r="AE83" s="12"/>
+      <c r="AF83" s="12"/>
+      <c r="AH83" s="30">
+        <f>(AE82-AC83)/AE82*100</f>
+        <v>0.51020408163266029</v>
+      </c>
+      <c r="AI83" s="30">
+        <f>(AD83-AF82)/AF82*100</f>
+        <v>3.9434961742201264</v>
+      </c>
+    </row>
+    <row r="86" spans="27:35" x14ac:dyDescent="0.45">
+      <c r="AC86" s="20"/>
+      <c r="AD86" s="20"/>
+      <c r="AE86" s="20"/>
+      <c r="AF86" s="20"/>
+      <c r="AG86" s="20"/>
+      <c r="AH86" s="20"/>
+    </row>
+    <row r="87" spans="27:35" x14ac:dyDescent="0.45">
+      <c r="AC87" s="20"/>
+      <c r="AD87" s="20"/>
+      <c r="AE87" s="20"/>
+      <c r="AF87" s="20"/>
+      <c r="AG87" s="20"/>
+      <c r="AH87" s="20"/>
+    </row>
+    <row r="88" spans="27:35" x14ac:dyDescent="0.45">
+      <c r="AC88" s="20"/>
+      <c r="AD88" s="20"/>
+      <c r="AE88" s="20"/>
+      <c r="AF88" s="20"/>
+      <c r="AG88" s="20"/>
+      <c r="AH88" s="20"/>
+    </row>
+    <row r="89" spans="27:35" x14ac:dyDescent="0.45">
+      <c r="AC89" s="20"/>
+      <c r="AD89" s="20"/>
+      <c r="AE89" s="20"/>
+      <c r="AF89" s="20"/>
+      <c r="AG89" s="20"/>
+      <c r="AH89" s="20"/>
+    </row>
+    <row r="90" spans="27:35" x14ac:dyDescent="0.45">
+      <c r="AC90" s="20"/>
+      <c r="AD90" s="20"/>
+      <c r="AE90" s="20"/>
+      <c r="AF90" s="20"/>
+      <c r="AG90" s="20"/>
+      <c r="AH90" s="20"/>
+    </row>
+    <row r="91" spans="27:35" x14ac:dyDescent="0.45">
+      <c r="AC91" s="20"/>
+      <c r="AD91" s="20"/>
+      <c r="AE91" s="20"/>
+      <c r="AF91" s="20"/>
+      <c r="AG91" s="20"/>
+      <c r="AH91" s="20"/>
+    </row>
+    <row r="92" spans="27:35" x14ac:dyDescent="0.45">
+      <c r="AC92" s="20"/>
+      <c r="AD92" s="20"/>
+      <c r="AE92" s="20"/>
+      <c r="AF92" s="20"/>
+      <c r="AG92" s="20"/>
+      <c r="AH92" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="22">
-    <mergeCell ref="V51:AC51"/>
+  <mergeCells count="29">
+    <mergeCell ref="AA83:AB83"/>
+    <mergeCell ref="AE82:AE83"/>
+    <mergeCell ref="AF82:AF83"/>
+    <mergeCell ref="AC80:AD80"/>
+    <mergeCell ref="AA82:AB82"/>
+    <mergeCell ref="AC79:AI79"/>
+    <mergeCell ref="E53:F53"/>
+    <mergeCell ref="H53:I53"/>
+    <mergeCell ref="K53:L53"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="J2:N2"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="M3:N3"/>
     <mergeCell ref="V52:W52"/>
     <mergeCell ref="Y52:Z52"/>
     <mergeCell ref="AB52:AC52"/>
@@ -6892,20 +7921,13 @@
     <mergeCell ref="AA3:AB3"/>
     <mergeCell ref="AD3:AE3"/>
     <mergeCell ref="E52:L52"/>
-    <mergeCell ref="E53:F53"/>
-    <mergeCell ref="H53:I53"/>
-    <mergeCell ref="K53:L53"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="J2:N2"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="V51:AI51"/>
+    <mergeCell ref="AG52:AH52"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
-  <tableParts count="14">
+  <tableParts count="15">
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
@@ -6920,6 +7942,7 @@
     <tablePart r:id="rId14"/>
     <tablePart r:id="rId15"/>
     <tablePart r:id="rId16"/>
+    <tablePart r:id="rId17"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>